<commit_message>
Add 3 first test case
</commit_message>
<xml_diff>
--- a/test_case_v2.xlsx
+++ b/test_case_v2.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nguyen Duong\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\20181\QLDACNTT\BTL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BB85DFB8-D4AC-4075-B003-CFA54E7D1638}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" tabRatio="865" activeTab="2" xr2:uid="{4F073D21-8F2D-40FD-8838-9512BCF003D6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" tabRatio="865" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Mô tả chung" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
     <sheet name="LưuƯV" sheetId="13" r:id="rId11"/>
     <sheet name="ĐánhGiáBĐ" sheetId="14" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -926,8 +925,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -970,12 +969,6 @@
       <color indexed="9"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="2"/>
-      <charset val="128"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1468,7 +1461,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="71">
+  <cellStyleXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1495,51 +1488,50 @@
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1588,65 +1580,65 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="8" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="9" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="8" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="9" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="10" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="10" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="11" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="11" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="11" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="11" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="12" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="12" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="13" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="13" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="14" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="13" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="15" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="16" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="8" xfId="27" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="17" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="14" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="13" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="15" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="16" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="8" xfId="27" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="17" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="18" xfId="27" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="19" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="18" xfId="27" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="19" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="14" fillId="23" borderId="0" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="13" fillId="23" borderId="0" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="14" fillId="23" borderId="0" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="13" fillId="23" borderId="0" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="18" fillId="23" borderId="0" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="17" fillId="23" borderId="0" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="28"/>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="20" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="20" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="70" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="69" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1655,9 +1647,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1744,7 +1736,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1772,78 +1764,77 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="71">
-    <cellStyle name="20% - Accent1 2" xfId="2" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="20% - Accent2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
-    <cellStyle name="20% - Accent3 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="20% - Accent4 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="20% - Accent5 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="20% - Accent6 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
-    <cellStyle name="40% - Accent1 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="40% - Accent2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="40% - Accent3 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="40% - Accent4 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="40% - Accent5 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
-    <cellStyle name="40% - Accent6 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
-    <cellStyle name="60% - Accent1 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="60% - Accent2 2" xfId="15" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="60% - Accent3 2" xfId="16" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
-    <cellStyle name="60% - Accent4 2" xfId="17" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
-    <cellStyle name="60% - Accent5 2" xfId="18" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
-    <cellStyle name="60% - Accent6 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
-    <cellStyle name="Accent1 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
-    <cellStyle name="Accent2 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
-    <cellStyle name="Accent3 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
-    <cellStyle name="Accent4 2" xfId="23" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
-    <cellStyle name="Accent5 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
-    <cellStyle name="Accent6 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
-    <cellStyle name="Bình thường 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
-    <cellStyle name="Bình thường 3" xfId="69" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
-    <cellStyle name="Hyperlink 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
-    <cellStyle name="Normal 2" xfId="27" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
-    <cellStyle name="Normal 3" xfId="28" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
-    <cellStyle name="Normal 4 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="Normal 4 3" xfId="30" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
-    <cellStyle name="Normal_Sheet1" xfId="31" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
-    <cellStyle name="Note 10" xfId="32" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="Note 10 2" xfId="33" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="Note 10 3" xfId="34" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="Note 11" xfId="35" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
-    <cellStyle name="Note 11 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
-    <cellStyle name="Note 11 3" xfId="37" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
-    <cellStyle name="Note 12" xfId="38" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
-    <cellStyle name="Note 12 2" xfId="39" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
-    <cellStyle name="Note 12 3" xfId="40" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
-    <cellStyle name="Note 13" xfId="41" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="Note 14" xfId="42" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
-    <cellStyle name="Note 15" xfId="43" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
-    <cellStyle name="Note 2" xfId="44" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
-    <cellStyle name="Note 2 2" xfId="45" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
-    <cellStyle name="Note 2 3" xfId="46" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
-    <cellStyle name="Note 3" xfId="47" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
-    <cellStyle name="Note 3 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
-    <cellStyle name="Note 3 3" xfId="49" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
-    <cellStyle name="Note 4" xfId="50" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
-    <cellStyle name="Note 4 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
-    <cellStyle name="Note 4 3" xfId="52" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
-    <cellStyle name="Note 5" xfId="53" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
-    <cellStyle name="Note 5 2" xfId="54" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
-    <cellStyle name="Note 5 3" xfId="55" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
-    <cellStyle name="Note 6" xfId="56" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
-    <cellStyle name="Note 6 2" xfId="57" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
-    <cellStyle name="Note 6 3" xfId="58" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
-    <cellStyle name="Note 7" xfId="59" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
-    <cellStyle name="Note 7 2" xfId="60" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
-    <cellStyle name="Note 7 3" xfId="61" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
-    <cellStyle name="Note 8" xfId="62" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
-    <cellStyle name="Note 8 2" xfId="63" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
-    <cellStyle name="Note 8 3" xfId="64" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
-    <cellStyle name="Note 9" xfId="65" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
-    <cellStyle name="Note 9 2" xfId="66" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
-    <cellStyle name="Note 9 3" xfId="67" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
-    <cellStyle name="Siêu kết nối" xfId="70" builtinId="8"/>
-    <cellStyle name="標準_結合試験(AllOvertheWorld)" xfId="68" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
+  <cellStyles count="70">
+    <cellStyle name="20% - Accent1 2" xfId="2"/>
+    <cellStyle name="20% - Accent2 2" xfId="3"/>
+    <cellStyle name="20% - Accent3 2" xfId="4"/>
+    <cellStyle name="20% - Accent4 2" xfId="5"/>
+    <cellStyle name="20% - Accent5 2" xfId="6"/>
+    <cellStyle name="20% - Accent6 2" xfId="7"/>
+    <cellStyle name="40% - Accent1 2" xfId="8"/>
+    <cellStyle name="40% - Accent2 2" xfId="9"/>
+    <cellStyle name="40% - Accent3 2" xfId="10"/>
+    <cellStyle name="40% - Accent4 2" xfId="11"/>
+    <cellStyle name="40% - Accent5 2" xfId="12"/>
+    <cellStyle name="40% - Accent6 2" xfId="13"/>
+    <cellStyle name="60% - Accent1 2" xfId="14"/>
+    <cellStyle name="60% - Accent2 2" xfId="15"/>
+    <cellStyle name="60% - Accent3 2" xfId="16"/>
+    <cellStyle name="60% - Accent4 2" xfId="17"/>
+    <cellStyle name="60% - Accent5 2" xfId="18"/>
+    <cellStyle name="60% - Accent6 2" xfId="19"/>
+    <cellStyle name="Accent1 2" xfId="20"/>
+    <cellStyle name="Accent2 2" xfId="21"/>
+    <cellStyle name="Accent3 2" xfId="22"/>
+    <cellStyle name="Accent4 2" xfId="23"/>
+    <cellStyle name="Accent5 2" xfId="24"/>
+    <cellStyle name="Accent6 2" xfId="25"/>
+    <cellStyle name="Bình thường 2" xfId="1"/>
+    <cellStyle name="Bình thường 3" xfId="68"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8"/>
+    <cellStyle name="Hyperlink 2" xfId="26"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="27"/>
+    <cellStyle name="Normal 3" xfId="28"/>
+    <cellStyle name="Normal 4 2" xfId="29"/>
+    <cellStyle name="Normal 4 3" xfId="30"/>
+    <cellStyle name="Note 10" xfId="31"/>
+    <cellStyle name="Note 10 2" xfId="32"/>
+    <cellStyle name="Note 10 3" xfId="33"/>
+    <cellStyle name="Note 11" xfId="34"/>
+    <cellStyle name="Note 11 2" xfId="35"/>
+    <cellStyle name="Note 11 3" xfId="36"/>
+    <cellStyle name="Note 12" xfId="37"/>
+    <cellStyle name="Note 12 2" xfId="38"/>
+    <cellStyle name="Note 12 3" xfId="39"/>
+    <cellStyle name="Note 13" xfId="40"/>
+    <cellStyle name="Note 14" xfId="41"/>
+    <cellStyle name="Note 15" xfId="42"/>
+    <cellStyle name="Note 2" xfId="43"/>
+    <cellStyle name="Note 2 2" xfId="44"/>
+    <cellStyle name="Note 2 3" xfId="45"/>
+    <cellStyle name="Note 3" xfId="46"/>
+    <cellStyle name="Note 3 2" xfId="47"/>
+    <cellStyle name="Note 3 3" xfId="48"/>
+    <cellStyle name="Note 4" xfId="49"/>
+    <cellStyle name="Note 4 2" xfId="50"/>
+    <cellStyle name="Note 4 3" xfId="51"/>
+    <cellStyle name="Note 5" xfId="52"/>
+    <cellStyle name="Note 5 2" xfId="53"/>
+    <cellStyle name="Note 5 3" xfId="54"/>
+    <cellStyle name="Note 6" xfId="55"/>
+    <cellStyle name="Note 6 2" xfId="56"/>
+    <cellStyle name="Note 6 3" xfId="57"/>
+    <cellStyle name="Note 7" xfId="58"/>
+    <cellStyle name="Note 7 2" xfId="59"/>
+    <cellStyle name="Note 7 3" xfId="60"/>
+    <cellStyle name="Note 8" xfId="61"/>
+    <cellStyle name="Note 8 2" xfId="62"/>
+    <cellStyle name="Note 8 3" xfId="63"/>
+    <cellStyle name="Note 9" xfId="64"/>
+    <cellStyle name="Note 9 2" xfId="65"/>
+    <cellStyle name="Note 9 3" xfId="66"/>
+    <cellStyle name="標準_結合試験(AllOvertheWorld)" xfId="67"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2154,7 +2145,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FE9FCA4-BEB0-468F-BC62-981B610970DB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2266,7 +2257,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD045726-E3FA-42F1-A8D4-5C3FB41FF7E6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L22"/>
   <sheetViews>
     <sheetView topLeftCell="B13" workbookViewId="0">
@@ -2707,7 +2698,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7646FC00-93F9-4B5B-9602-2FF66E1DF449}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L20"/>
   <sheetViews>
     <sheetView topLeftCell="D10" workbookViewId="0">
@@ -3057,7 +3048,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{830B3A08-772F-44A0-B7FC-239E765BF48A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L20"/>
   <sheetViews>
     <sheetView topLeftCell="D7" workbookViewId="0">
@@ -3407,7 +3398,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD70E22-ACCB-47A3-B744-68D84D3695CC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F17"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -3646,17 +3637,17 @@
     <mergeCell ref="B2:E2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D7" location="'QTHT_DangNhap-DangXuat'!A1" display="QTHT_DangNhap-DangXuat" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="D7" location="'QTHT_DangNhap-DangXuat'!A1" display="QTHT_DangNhap-DangXuat"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0C936BD-71B4-4B6E-AE8C-1BBC9E6AF92E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -4282,11 +4273,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA41520-62E0-4A12-9F18-4AC657220892}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L20"/>
   <sheetViews>
     <sheetView topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4655,7 +4646,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A5526D5-1EFA-482A-A5B6-01599D2C331D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5028,7 +5019,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E8E07A-32EF-4945-9A29-CC137F516B58}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L20"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -5355,10 +5346,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF15AEA9-C21F-4AD3-B468-E26FF260BAFE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L20"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
@@ -5734,7 +5725,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AF418F-B4EE-4DBE-99D8-310F59B8923A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L19"/>
   <sheetViews>
     <sheetView topLeftCell="E10" workbookViewId="0">
@@ -6104,7 +6095,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACC43551-78B3-4B2C-8D32-DF0E14D15E1E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L20"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">

</xml_diff>